<commit_message>
docs: add revised user stories (V2) with updated story points and hours
</commit_message>
<xml_diff>
--- a/docs/UserStories/UserStories.xlsx
+++ b/docs/UserStories/UserStories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maila/Desktop/ProjektSchule/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maila/Desktop/ProjektSchule/Werkzeugsverwaltungstool/docs/UserStories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0593202E-8C45-044E-9A3B-5306D231053D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCBA89-DC56-0146-9C93-CF708EC48D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,9 +316,6 @@
 - Detailansicht zeigt Verlauf der Anfrage/Entscheidung</t>
   </si>
   <si>
-    <t>die Ausleihhistorie eines Mitarbeiters/Auszubildender einsehen</t>
-  </si>
-  <si>
     <t>- Rückgabe wird erfasst, beendet Ausleihe und ändert wieder den Status
 - Zustand bei Rückgabe dokumentieren
 - Bei „defekt“ wird Werkzeugstatus auf „defekt“ gesetzt</t>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Admin / Abteilungsleiter</t>
+  </si>
+  <si>
+    <t>die Ausleihhistorie eines Mitarbeiters einsehen</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +413,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -442,11 +448,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -470,6 +491,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -938,77 +966,77 @@
       </c>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="3:15" ht="64" x14ac:dyDescent="0.2">
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="3:15" s="15" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="C4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="16">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="16">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="16">
         <v>5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="16">
         <v>2</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="3:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="C5" s="5" t="s">
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="3:15" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="C5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="16">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="16">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="16">
         <v>5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="16">
         <v>2</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O5" s="5"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="3:15" ht="80" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
@@ -1346,7 +1374,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>36</v>
@@ -1358,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="3:15" ht="64" x14ac:dyDescent="0.2">
@@ -1378,7 +1406,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>38</v>
@@ -1393,7 +1421,7 @@
         <v>4</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="3:15" ht="64" x14ac:dyDescent="0.2">
@@ -1416,7 +1444,7 @@
         <v>27</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>41</v>
@@ -1463,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="3:15" ht="64" x14ac:dyDescent="0.2">
@@ -1498,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O19" s="5"/>
     </row>

</xml_diff>